<commit_message>
Swedish steel and simplex method
</commit_message>
<xml_diff>
--- a/Python/Swedish_steel_IPM.xlsx
+++ b/Python/Swedish_steel_IPM.xlsx
@@ -382,15 +382,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -412,11 +412,11 @@
       <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" t="s">
+      <c r="R1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -439,93 +439,213 @@
         <v>1</v>
       </c>
       <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+      <c r="B3">
+        <v>-7.0000000000000001E-3</v>
+      </c>
+      <c r="C3">
+        <v>-8.5000000000000006E-3</v>
+      </c>
+      <c r="D3">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>-6.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="B4">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="C4">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="D4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>-0.18</v>
+      </c>
+      <c r="B5">
+        <v>-3.2000000000000001E-2</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
         <v>-1</v>
       </c>
-      <c r="B3">
-        <v>-1</v>
-      </c>
-      <c r="C3">
-        <v>-1</v>
-      </c>
-      <c r="D3">
-        <v>-1</v>
-      </c>
-      <c r="E3">
-        <v>-1</v>
-      </c>
-      <c r="F3">
-        <v>-1</v>
-      </c>
-      <c r="G3">
-        <v>-1</v>
-      </c>
-      <c r="H3">
-        <v>-1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>-8.0000000000000002E-3</v>
-      </c>
-      <c r="B4">
-        <v>-7.0000000000000001E-3</v>
-      </c>
-      <c r="C4">
-        <v>-8.5000000000000006E-3</v>
-      </c>
-      <c r="D4">
-        <v>-4.0000000000000001E-3</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>-6.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="B5">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="C5">
-        <v>8.5000000000000006E-3</v>
-      </c>
-      <c r="D5">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5" s="1">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>-0.18</v>
+        <v>0.18</v>
       </c>
       <c r="B6">
-        <v>-3.2000000000000001E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -534,7 +654,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -543,44 +663,104 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>-30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>0.18</v>
-      </c>
-      <c r="B7">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8">
         <f>-12/100</f>
         <v>-0.12</v>
       </c>
-      <c r="B8">
+      <c r="B7">
         <f>-1.1/100</f>
         <v>-1.1000000000000001E-2</v>
       </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>-1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0.12</v>
+      </c>
+      <c r="B8">
+        <v>1.0999999999999999E-2</v>
+      </c>
       <c r="C8">
         <v>0</v>
       </c>
@@ -591,47 +771,107 @@
         <v>0</v>
       </c>
       <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>-1E-3</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
         <v>-1</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>0.12</v>
-      </c>
-      <c r="B9">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
       <c r="H9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0</v>
       </c>
       <c r="B10">
-        <v>-1E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -646,18 +886,48 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>-11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -672,18 +942,48 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -701,32 +1001,36 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>0</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
         <v>250</v>
       </c>
     </row>

</xml_diff>